<commit_message>
User story 8 updated
</commit_message>
<xml_diff>
--- a/Sprint 2/Sprint_Backlog/Sprint2Backlog.xlsx
+++ b/Sprint 2/Sprint_Backlog/Sprint2Backlog.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22325"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arnavdhawan\Desktop\Sprint 2\Sprint_Backlog\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\antho\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3CE42C87-635E-434E-9082-8C1C9B069B2B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" tabRatio="500"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Agile Sprint Backlog" sheetId="5" r:id="rId1"/>
@@ -20,12 +21,20 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Agile Sprint Backlog'!$B$2:$W$28</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Agile Sprint Backlog - BLANK'!$B$2:$V$28</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="61">
   <si>
     <t>User Story #1</t>
   </si>
@@ -206,11 +215,14 @@
   <si>
     <t>To Do</t>
   </si>
+  <si>
+    <t>In testing</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -381,18 +393,18 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -454,7 +466,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -505,13 +516,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -674,7 +685,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1304,19 +1314,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="B1:AC148"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.25" style="3" customWidth="1"/>
     <col min="2" max="2" width="34.75" style="3" customWidth="1"/>
@@ -1335,31 +1345,31 @@
     <col min="25" max="16384" width="10.75" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:29" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B1" s="12" t="s">
+    <row r="1" spans="2:29" ht="49.9" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="B1" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13"/>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="13"/>
-      <c r="S1" s="13"/>
-      <c r="T1" s="13"/>
-      <c r="U1" s="13"/>
-      <c r="V1" s="13"/>
-      <c r="W1" s="13"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+      <c r="S1" s="14"/>
+      <c r="T1" s="14"/>
+      <c r="U1" s="14"/>
+      <c r="V1" s="14"/>
+      <c r="W1" s="14"/>
       <c r="X1" s="4"/>
       <c r="Y1" s="4"/>
       <c r="Z1" s="4"/>
@@ -1885,7 +1895,7 @@
       <c r="AB12" s="4"/>
       <c r="AC12" s="4"/>
     </row>
-    <row r="13" spans="2:29" ht="51" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:29" ht="37.5" x14ac:dyDescent="0.25">
       <c r="B13" s="7" t="s">
         <v>24</v>
       </c>
@@ -2115,7 +2125,7 @@
       <c r="AB17" s="4"/>
       <c r="AC17" s="4"/>
     </row>
-    <row r="18" spans="2:29" ht="51" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:29" ht="37.5" x14ac:dyDescent="0.25">
       <c r="B18" s="7" t="s">
         <v>30</v>
       </c>
@@ -2347,7 +2357,7 @@
       <c r="AB22" s="4"/>
       <c r="AC22" s="4"/>
     </row>
-    <row r="23" spans="2:29" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:29" ht="37.5" x14ac:dyDescent="0.25">
       <c r="B23" s="7" t="s">
         <v>37</v>
       </c>
@@ -2575,7 +2585,7 @@
       <c r="AB27" s="4"/>
       <c r="AC27" s="4"/>
     </row>
-    <row r="28" spans="2:29" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:29" ht="37.5" x14ac:dyDescent="0.25">
       <c r="B28" s="7" t="s">
         <v>41</v>
       </c>
@@ -2609,7 +2619,7 @@
       <c r="AB28" s="4"/>
       <c r="AC28" s="4"/>
     </row>
-    <row r="29" spans="2:29" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:29" ht="37.5" x14ac:dyDescent="0.25">
       <c r="B29" s="9" t="s">
         <v>40</v>
       </c>
@@ -2694,16 +2704,16 @@
       <c r="M30" s="9">
         <v>0</v>
       </c>
-      <c r="N30" s="14"/>
-      <c r="O30" s="14"/>
-      <c r="P30" s="14"/>
-      <c r="Q30" s="14"/>
-      <c r="R30" s="14"/>
-      <c r="S30" s="14"/>
-      <c r="T30" s="14"/>
-      <c r="U30" s="14"/>
-      <c r="V30" s="14"/>
-      <c r="W30" s="14"/>
+      <c r="N30" s="12"/>
+      <c r="O30" s="12"/>
+      <c r="P30" s="12"/>
+      <c r="Q30" s="12"/>
+      <c r="R30" s="12"/>
+      <c r="S30" s="12"/>
+      <c r="T30" s="12"/>
+      <c r="U30" s="12"/>
+      <c r="V30" s="12"/>
+      <c r="W30" s="12"/>
       <c r="X30" s="4"/>
       <c r="Y30" s="4"/>
       <c r="Z30" s="4"/>
@@ -2803,7 +2813,7 @@
       <c r="AB32" s="4"/>
       <c r="AC32" s="4"/>
     </row>
-    <row r="33" spans="2:29" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:29" ht="25" x14ac:dyDescent="0.25">
       <c r="B33" s="7" t="s">
         <v>43</v>
       </c>
@@ -2837,7 +2847,7 @@
       <c r="AB33" s="4"/>
       <c r="AC33" s="4"/>
     </row>
-    <row r="34" spans="2:29" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:29" ht="37.5" x14ac:dyDescent="0.25">
       <c r="B34" s="9" t="s">
         <v>42</v>
       </c>
@@ -2847,16 +2857,16 @@
       </c>
       <c r="E34" s="9"/>
       <c r="F34" s="9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G34" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H34" s="9">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I34" s="9">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="J34" s="9">
         <v>0</v>
@@ -3031,7 +3041,7 @@
       <c r="AB37" s="4"/>
       <c r="AC37" s="4"/>
     </row>
-    <row r="38" spans="2:29" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:29" ht="37.5" x14ac:dyDescent="0.25">
       <c r="B38" s="7" t="s">
         <v>45</v>
       </c>
@@ -3067,7 +3077,7 @@
       <c r="AB38" s="4"/>
       <c r="AC38" s="4"/>
     </row>
-    <row r="39" spans="2:29" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:29" ht="37.5" x14ac:dyDescent="0.25">
       <c r="B39" s="9" t="s">
         <v>47</v>
       </c>
@@ -3255,7 +3265,7 @@
       <c r="AB42" s="4"/>
       <c r="AC42" s="4"/>
     </row>
-    <row r="43" spans="2:29" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:29" ht="37.5" x14ac:dyDescent="0.25">
       <c r="B43" s="7" t="s">
         <v>46</v>
       </c>
@@ -3477,7 +3487,7 @@
       <c r="AB47" s="4"/>
       <c r="AC47" s="4"/>
     </row>
-    <row r="48" spans="2:29" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:29" ht="25" x14ac:dyDescent="0.25">
       <c r="B48" s="7" t="s">
         <v>50</v>
       </c>
@@ -3713,15 +3723,15 @@
       <c r="F53" s="5"/>
       <c r="G53" s="5">
         <f>SUM(G3:G52)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H53" s="5">
         <f>SUM(H4:H52)</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I53" s="5">
         <f>SUM(I3:I52)</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="J53" s="5">
         <f>SUM(J3:J52)</f>
@@ -6217,7 +6227,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="3" tint="0.39997558519241921"/>
     <pageSetUpPr fitToPage="1"/>
@@ -6229,7 +6239,7 @@
       <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.25" style="3" customWidth="1"/>
     <col min="2" max="2" width="34.75" style="3" customWidth="1"/>
@@ -6247,30 +6257,30 @@
     <col min="24" max="16384" width="10.75" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:28" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B1" s="12" t="s">
+    <row r="1" spans="2:28" ht="49.9" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="B1" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13"/>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="13"/>
-      <c r="S1" s="13"/>
-      <c r="T1" s="13"/>
-      <c r="U1" s="13"/>
-      <c r="V1" s="13"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+      <c r="S1" s="14"/>
+      <c r="T1" s="14"/>
+      <c r="U1" s="14"/>
+      <c r="V1" s="14"/>
       <c r="W1" s="4"/>
       <c r="X1" s="4"/>
       <c r="Y1" s="4"/>
@@ -9922,7 +9932,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="1"/>
   </sheetPr>
@@ -9932,14 +9942,14 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="3.25" style="11" customWidth="1"/>
     <col min="2" max="2" width="88.25" style="11" customWidth="1"/>
     <col min="3" max="16384" width="10.75" style="11"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:2" ht="93" x14ac:dyDescent="0.35">
       <c r="B2" s="10" t="s">
         <v>20</v>
       </c>

</xml_diff>

<commit_message>
Changes made to user story #9
</commit_message>
<xml_diff>
--- a/Sprint 2/Sprint_Backlog/Sprint2Backlog.xlsx
+++ b/Sprint 2/Sprint_Backlog/Sprint2Backlog.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22325"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\antho\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\afzalmiah\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3CE42C87-635E-434E-9082-8C1C9B069B2B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Agile Sprint Backlog" sheetId="5" r:id="rId1"/>
@@ -21,7 +20,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Agile Sprint Backlog'!$B$2:$W$28</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Agile Sprint Backlog - BLANK'!$B$2:$V$28</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="64">
   <si>
     <t>User Story #1</t>
   </si>
@@ -180,9 +179,6 @@
     <t>1. Format website to accommodate the map filters and data on the same page.</t>
   </si>
   <si>
-    <t>1. Format the website to include two search box, one for code and one for procedure.</t>
-  </si>
-  <si>
     <t>Anthony</t>
   </si>
   <si>
@@ -218,11 +214,23 @@
   <si>
     <t>In testing</t>
   </si>
+  <si>
+    <t>Development</t>
+  </si>
+  <si>
+    <t>2. validate the two search boxes to disallow a search when both search boxes are not null</t>
+  </si>
+  <si>
+    <t>3. Modify layout to have search bars side by side with buttons underneath</t>
+  </si>
+  <si>
+    <t>1. Format the website to include two search box, one for code and one for procedure with each search box returning entries</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -404,7 +412,7 @@
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -466,6 +474,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -516,13 +525,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.5</c:v>
+                  <c:v>4.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -902,51 +911,6 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>25400</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>45156</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>15320</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E346FCE9-8543-7647-9B03-5B2850F609DC}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="18034000" y="0"/>
-          <a:ext cx="3321756" cy="650320"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1314,19 +1278,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="B1:AC148"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M4" sqref="M4"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.25" style="3" customWidth="1"/>
     <col min="2" max="2" width="34.75" style="3" customWidth="1"/>
@@ -1345,7 +1309,7 @@
     <col min="25" max="16384" width="10.75" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:29" ht="49.9" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="1" spans="2:29" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B1" s="13" t="s">
         <v>44</v>
       </c>
@@ -1388,7 +1352,7 @@
         <v>10</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>11</v>
@@ -1471,11 +1435,11 @@
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E4" s="9"/>
       <c r="F4" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G4" s="9">
         <v>0</v>
@@ -1521,11 +1485,11 @@
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E5" s="9"/>
       <c r="F5" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G5" s="9">
         <v>0</v>
@@ -1571,11 +1535,11 @@
       </c>
       <c r="C6" s="9"/>
       <c r="D6" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E6" s="9"/>
       <c r="F6" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G6" s="9">
         <v>0</v>
@@ -1703,13 +1667,13 @@
       </c>
       <c r="C9" s="9"/>
       <c r="D9" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G9" s="9">
         <v>0</v>
@@ -1755,11 +1719,11 @@
       </c>
       <c r="C10" s="9"/>
       <c r="D10" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E10" s="9"/>
       <c r="F10" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G10" s="9">
         <v>0</v>
@@ -1805,11 +1769,11 @@
       </c>
       <c r="C11" s="9"/>
       <c r="D11" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E11" s="9"/>
       <c r="F11" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G11" s="9">
         <v>0</v>
@@ -1895,7 +1859,7 @@
       <c r="AB12" s="4"/>
       <c r="AC12" s="4"/>
     </row>
-    <row r="13" spans="2:29" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:29" ht="51" x14ac:dyDescent="0.25">
       <c r="B13" s="7" t="s">
         <v>24</v>
       </c>
@@ -1935,11 +1899,11 @@
       </c>
       <c r="C14" s="9"/>
       <c r="D14" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E14" s="9"/>
       <c r="F14" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G14" s="9">
         <v>0</v>
@@ -1985,11 +1949,11 @@
       </c>
       <c r="C15" s="9"/>
       <c r="D15" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E15" s="9"/>
       <c r="F15" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G15" s="9">
         <v>0</v>
@@ -2035,11 +1999,11 @@
       </c>
       <c r="C16" s="9"/>
       <c r="D16" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E16" s="9"/>
       <c r="F16" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G16" s="9">
         <v>0</v>
@@ -2125,7 +2089,7 @@
       <c r="AB17" s="4"/>
       <c r="AC17" s="4"/>
     </row>
-    <row r="18" spans="2:29" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:29" ht="51" x14ac:dyDescent="0.25">
       <c r="B18" s="7" t="s">
         <v>30</v>
       </c>
@@ -2165,13 +2129,13 @@
       </c>
       <c r="C19" s="9"/>
       <c r="D19" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G19" s="9">
         <v>0</v>
@@ -2217,11 +2181,11 @@
       </c>
       <c r="C20" s="9"/>
       <c r="D20" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E20" s="9"/>
       <c r="F20" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G20" s="9">
         <v>0</v>
@@ -2267,11 +2231,11 @@
       </c>
       <c r="C21" s="9"/>
       <c r="D21" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E21" s="9"/>
       <c r="F21" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G21" s="9">
         <v>0</v>
@@ -2357,7 +2321,7 @@
       <c r="AB22" s="4"/>
       <c r="AC22" s="4"/>
     </row>
-    <row r="23" spans="2:29" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:29" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B23" s="7" t="s">
         <v>37</v>
       </c>
@@ -2397,13 +2361,13 @@
       </c>
       <c r="C24" s="9"/>
       <c r="D24" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F24" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G24" s="9">
         <v>0</v>
@@ -2449,11 +2413,11 @@
       </c>
       <c r="C25" s="9"/>
       <c r="D25" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E25" s="9"/>
       <c r="F25" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G25" s="9">
         <v>0</v>
@@ -2585,7 +2549,7 @@
       <c r="AB27" s="4"/>
       <c r="AC27" s="4"/>
     </row>
-    <row r="28" spans="2:29" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:29" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B28" s="7" t="s">
         <v>41</v>
       </c>
@@ -2619,19 +2583,19 @@
       <c r="AB28" s="4"/>
       <c r="AC28" s="4"/>
     </row>
-    <row r="29" spans="2:29" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:29" ht="40.5" x14ac:dyDescent="0.25">
       <c r="B29" s="9" t="s">
         <v>40</v>
       </c>
       <c r="C29" s="9"/>
       <c r="D29" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F29" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G29" s="9">
         <v>0</v>
@@ -2677,11 +2641,11 @@
       </c>
       <c r="C30" s="9"/>
       <c r="D30" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E30" s="9"/>
       <c r="F30" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G30" s="9">
         <v>0</v>
@@ -2813,7 +2777,7 @@
       <c r="AB32" s="4"/>
       <c r="AC32" s="4"/>
     </row>
-    <row r="33" spans="2:29" ht="25" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:29" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B33" s="7" t="s">
         <v>43</v>
       </c>
@@ -2847,17 +2811,17 @@
       <c r="AB33" s="4"/>
       <c r="AC33" s="4"/>
     </row>
-    <row r="34" spans="2:29" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:29" ht="40.5" x14ac:dyDescent="0.25">
       <c r="B34" s="9" t="s">
         <v>42</v>
       </c>
       <c r="C34" s="9"/>
       <c r="D34" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E34" s="9"/>
       <c r="F34" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G34" s="9">
         <v>1</v>
@@ -2905,7 +2869,7 @@
       <c r="D35" s="9"/>
       <c r="E35" s="9"/>
       <c r="F35" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G35" s="9">
         <v>0</v>
@@ -2953,7 +2917,7 @@
       <c r="D36" s="9"/>
       <c r="E36" s="9"/>
       <c r="F36" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G36" s="9">
         <v>0</v>
@@ -3001,7 +2965,7 @@
       <c r="D37" s="9"/>
       <c r="E37" s="9"/>
       <c r="F37" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G37" s="9">
         <v>0</v>
@@ -3041,7 +3005,7 @@
       <c r="AB37" s="4"/>
       <c r="AC37" s="4"/>
     </row>
-    <row r="38" spans="2:29" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:29" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B38" s="7" t="s">
         <v>45</v>
       </c>
@@ -3051,7 +3015,7 @@
       <c r="D38" s="8"/>
       <c r="E38" s="8"/>
       <c r="F38" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G38" s="8"/>
       <c r="H38" s="8"/>
@@ -3077,17 +3041,17 @@
       <c r="AB38" s="4"/>
       <c r="AC38" s="4"/>
     </row>
-    <row r="39" spans="2:29" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:29" ht="40.5" x14ac:dyDescent="0.25">
       <c r="B39" s="9" t="s">
         <v>47</v>
       </c>
       <c r="C39" s="9"/>
       <c r="D39" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E39" s="9"/>
       <c r="F39" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G39" s="9">
         <v>0</v>
@@ -3265,7 +3229,7 @@
       <c r="AB42" s="4"/>
       <c r="AC42" s="4"/>
     </row>
-    <row r="43" spans="2:29" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:29" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B43" s="7" t="s">
         <v>46</v>
       </c>
@@ -3274,7 +3238,9 @@
       </c>
       <c r="D43" s="8"/>
       <c r="E43" s="8"/>
-      <c r="F43" s="9"/>
+      <c r="F43" s="9" t="s">
+        <v>60</v>
+      </c>
       <c r="G43" s="8"/>
       <c r="H43" s="8"/>
       <c r="I43" s="8"/>
@@ -3299,26 +3265,26 @@
       <c r="AB43" s="4"/>
       <c r="AC43" s="4"/>
     </row>
-    <row r="44" spans="2:29" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:29" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="9" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="C44" s="9"/>
       <c r="D44" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E44" s="9"/>
       <c r="F44" s="9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G44" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H44" s="9">
         <v>0</v>
       </c>
       <c r="I44" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J44" s="9">
         <v>0</v>
@@ -3349,22 +3315,26 @@
       <c r="AB44" s="4"/>
       <c r="AC44" s="4"/>
     </row>
-    <row r="45" spans="2:29" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:29" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C45" s="9"/>
+      <c r="D45" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E45" s="9"/>
+      <c r="F45" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="G45" s="9">
+        <v>3</v>
+      </c>
+      <c r="H45" s="9">
+        <v>0</v>
+      </c>
+      <c r="I45" s="9">
         <v>2</v>
-      </c>
-      <c r="C45" s="9"/>
-      <c r="D45" s="9"/>
-      <c r="E45" s="9"/>
-      <c r="F45" s="9"/>
-      <c r="G45" s="9">
-        <v>0</v>
-      </c>
-      <c r="H45" s="9">
-        <v>0</v>
-      </c>
-      <c r="I45" s="9">
-        <v>0</v>
       </c>
       <c r="J45" s="9">
         <v>0</v>
@@ -3395,22 +3365,26 @@
       <c r="AB45" s="4"/>
       <c r="AC45" s="4"/>
     </row>
-    <row r="46" spans="2:29" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:29" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="9" t="s">
-        <v>2</v>
+        <v>62</v>
       </c>
       <c r="C46" s="9"/>
-      <c r="D46" s="9"/>
+      <c r="D46" s="9" t="s">
+        <v>51</v>
+      </c>
       <c r="E46" s="9"/>
-      <c r="F46" s="9"/>
+      <c r="F46" s="9" t="s">
+        <v>60</v>
+      </c>
       <c r="G46" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H46" s="9">
         <v>0</v>
       </c>
       <c r="I46" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J46" s="9">
         <v>0</v>
@@ -3487,9 +3461,9 @@
       <c r="AB47" s="4"/>
       <c r="AC47" s="4"/>
     </row>
-    <row r="48" spans="2:29" ht="25" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:29" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B48" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C48" s="7">
         <v>3</v>
@@ -3527,13 +3501,13 @@
       </c>
       <c r="C49" s="9"/>
       <c r="D49" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="E49" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="F49" s="9" t="s">
         <v>58</v>
-      </c>
-      <c r="E49" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="F49" s="9" t="s">
-        <v>59</v>
       </c>
       <c r="G49" s="9">
         <v>0</v>
@@ -3673,7 +3647,7 @@
       <c r="D52" s="9"/>
       <c r="E52" s="9"/>
       <c r="F52" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G52" s="9">
         <v>0</v>
@@ -3723,7 +3697,7 @@
       <c r="F53" s="5"/>
       <c r="G53" s="5">
         <f>SUM(G3:G52)</f>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="H53" s="5">
         <f>SUM(H4:H52)</f>
@@ -3731,7 +3705,7 @@
       </c>
       <c r="I53" s="5">
         <f>SUM(I3:I52)</f>
-        <v>0.5</v>
+        <v>4.5</v>
       </c>
       <c r="J53" s="5">
         <f>SUM(J3:J52)</f>
@@ -6227,7 +6201,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3" tint="0.39997558519241921"/>
     <pageSetUpPr fitToPage="1"/>
@@ -6239,7 +6213,7 @@
       <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.25" style="3" customWidth="1"/>
     <col min="2" max="2" width="34.75" style="3" customWidth="1"/>
@@ -6257,7 +6231,7 @@
     <col min="24" max="16384" width="10.75" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:28" ht="49.9" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="1" spans="2:28" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B1" s="13" t="s">
         <v>7</v>
       </c>
@@ -9932,7 +9906,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="1"/>
   </sheetPr>
@@ -9942,14 +9916,14 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.25" style="11" customWidth="1"/>
     <col min="2" max="2" width="88.25" style="11" customWidth="1"/>
     <col min="3" max="16384" width="10.75" style="11"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" ht="93" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:2" ht="90" x14ac:dyDescent="0.25">
       <c r="B2" s="10" t="s">
         <v>20</v>
       </c>

</xml_diff>

<commit_message>
Updated with changes, addtions
</commit_message>
<xml_diff>
--- a/Sprint 2/Sprint_Backlog/Sprint2Backlog.xlsx
+++ b/Sprint 2/Sprint_Backlog/Sprint2Backlog.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="66">
   <si>
     <t>User Story #1</t>
   </si>
@@ -225,6 +225,12 @@
   </si>
   <si>
     <t>1. Format the website to include two search box, one for code and one for procedure with each search box returning entries</t>
+  </si>
+  <si>
+    <t>4. Validate the two search boxes to limit the input to only be either the code or description.</t>
+  </si>
+  <si>
+    <t>Testing</t>
   </si>
 </sst>
 </file>
@@ -1286,8 +1292,8 @@
   <dimension ref="B1:AC148"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F44" sqref="F44"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -1429,7 +1435,7 @@
       <c r="AB3" s="4"/>
       <c r="AC3" s="4"/>
     </row>
-    <row r="4" spans="2:29" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:29" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="9" t="s">
         <v>25</v>
       </c>
@@ -3275,7 +3281,7 @@
       </c>
       <c r="E44" s="9"/>
       <c r="F44" s="9" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="G44" s="9">
         <v>1</v>
@@ -3325,7 +3331,7 @@
       </c>
       <c r="E45" s="9"/>
       <c r="F45" s="9" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="G45" s="9">
         <v>3</v>
@@ -3375,7 +3381,7 @@
       </c>
       <c r="E46" s="9"/>
       <c r="F46" s="9" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="G46" s="9">
         <v>1</v>
@@ -3415,14 +3421,18 @@
       <c r="AB46" s="4"/>
       <c r="AC46" s="4"/>
     </row>
-    <row r="47" spans="2:29" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:29" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="9" t="s">
-        <v>2</v>
+        <v>64</v>
       </c>
       <c r="C47" s="9"/>
-      <c r="D47" s="9"/>
+      <c r="D47" s="9" t="s">
+        <v>51</v>
+      </c>
       <c r="E47" s="9"/>
-      <c r="F47" s="9"/>
+      <c r="F47" s="9" t="s">
+        <v>60</v>
+      </c>
       <c r="G47" s="9">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Updated User Story 1
</commit_message>
<xml_diff>
--- a/Sprint 2/Sprint_Backlog/Sprint2Backlog.xlsx
+++ b/Sprint 2/Sprint_Backlog/Sprint2Backlog.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\afzalmiah\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arnavdhawan\Desktop\Sprint 2\Sprint_Backlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -531,13 +531,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>6</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.5</c:v>
+                  <c:v>11.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -1292,8 +1292,8 @@
   <dimension ref="B1:AC148"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F46" sqref="F46"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9:F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -1406,7 +1406,7 @@
         <v>28</v>
       </c>
       <c r="C3" s="7">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
@@ -1445,16 +1445,16 @@
       </c>
       <c r="E4" s="9"/>
       <c r="F4" s="9" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G4" s="9">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H4" s="9">
         <v>0</v>
       </c>
       <c r="I4" s="9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J4" s="9">
         <v>0</v>
@@ -1495,16 +1495,16 @@
       </c>
       <c r="E5" s="9"/>
       <c r="F5" s="9" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G5" s="9">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="H5" s="9">
         <v>0</v>
       </c>
       <c r="I5" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J5" s="9">
         <v>0</v>
@@ -1548,7 +1548,7 @@
         <v>58</v>
       </c>
       <c r="G6" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H6" s="9">
         <v>0</v>
@@ -3707,7 +3707,7 @@
       <c r="F53" s="5"/>
       <c r="G53" s="5">
         <f>SUM(G3:G52)</f>
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="H53" s="5">
         <f>SUM(H4:H52)</f>
@@ -3715,7 +3715,7 @@
       </c>
       <c r="I53" s="5">
         <f>SUM(I3:I52)</f>
-        <v>4.5</v>
+        <v>11.5</v>
       </c>
       <c r="J53" s="5">
         <f>SUM(J3:J52)</f>

</xml_diff>

<commit_message>
Changes made to backlog
Issues moved to correct stage(Development or Testing or Review), User Story #9 - deleted unneeded task,
</commit_message>
<xml_diff>
--- a/Sprint 2/Sprint_Backlog/Sprint2Backlog.xlsx
+++ b/Sprint 2/Sprint_Backlog/Sprint2Backlog.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arnavdhawan\Desktop\Sprint 2\Sprint_Backlog\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\afzalmiah\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="67">
   <si>
     <t>User Story #1</t>
   </si>
@@ -128,9 +128,6 @@
     <t>User Story #4 As a website visitor, I want to see the list of hospitals based on the distance entered in the search box</t>
   </si>
   <si>
-    <t xml:space="preserve">3. Display the result received back to the user. </t>
-  </si>
-  <si>
     <t>3. Display the result received back to the user.</t>
   </si>
   <si>
@@ -138,9 +135,6 @@
   </si>
   <si>
     <t>3. Calculate distance.</t>
-  </si>
-  <si>
-    <t>2. Implement price filter.</t>
   </si>
   <si>
     <t>2. Implement distance filter.</t>
@@ -212,9 +206,6 @@
     <t>To Do</t>
   </si>
   <si>
-    <t>In testing</t>
-  </si>
-  <si>
     <t>Development</t>
   </si>
   <si>
@@ -230,7 +221,19 @@
     <t>4. Validate the two search boxes to limit the input to only be either the code or description.</t>
   </si>
   <si>
-    <t>Testing</t>
+    <t>In Review</t>
+  </si>
+  <si>
+    <t>Closed</t>
+  </si>
+  <si>
+    <t>In Development</t>
+  </si>
+  <si>
+    <t>1. Implement price filter.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. Display the result received back to the user. </t>
   </si>
 </sst>
 </file>
@@ -526,18 +529,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Agile Sprint Backlog'!$G$53:$M$53</c:f>
+              <c:f>'Agile Sprint Backlog'!$G$49:$M$49</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>26</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11.5</c:v>
+                  <c:v>15.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -1289,11 +1292,11 @@
     <tabColor theme="3"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:AC148"/>
+  <dimension ref="B1:AC144"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B9" sqref="B9:F10"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -1317,7 +1320,7 @@
   <sheetData>
     <row r="1" spans="2:29" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B1" s="13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C1" s="14"/>
       <c r="D1" s="14"/>
@@ -1358,7 +1361,7 @@
         <v>10</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>11</v>
@@ -1441,11 +1444,11 @@
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E4" s="9"/>
       <c r="F4" s="9" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G4" s="9">
         <v>4</v>
@@ -1491,11 +1494,11 @@
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E5" s="9"/>
       <c r="F5" s="9" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G5" s="9">
         <v>11</v>
@@ -1541,11 +1544,11 @@
       </c>
       <c r="C6" s="9"/>
       <c r="D6" s="9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E6" s="9"/>
       <c r="F6" s="9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G6" s="9">
         <v>5</v>
@@ -1673,13 +1676,13 @@
       </c>
       <c r="C9" s="9"/>
       <c r="D9" s="9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G9" s="9">
         <v>0</v>
@@ -1721,15 +1724,15 @@
     </row>
     <row r="10" spans="2:29" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C10" s="9"/>
       <c r="D10" s="9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E10" s="9"/>
       <c r="F10" s="9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G10" s="9">
         <v>0</v>
@@ -1771,15 +1774,15 @@
     </row>
     <row r="11" spans="2:29" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C11" s="9"/>
       <c r="D11" s="9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E11" s="9"/>
       <c r="F11" s="9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G11" s="9">
         <v>0</v>
@@ -1874,7 +1877,9 @@
       </c>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
-      <c r="F13" s="9"/>
+      <c r="F13" s="9" t="s">
+        <v>64</v>
+      </c>
       <c r="G13" s="8"/>
       <c r="H13" s="8"/>
       <c r="I13" s="8"/>
@@ -1901,18 +1906,18 @@
     </row>
     <row r="14" spans="2:29" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="9" t="s">
-        <v>22</v>
+        <v>65</v>
       </c>
       <c r="C14" s="9"/>
       <c r="D14" s="9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E14" s="9"/>
       <c r="F14" s="9" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="G14" s="9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H14" s="9">
         <v>0</v>
@@ -1951,18 +1956,18 @@
     </row>
     <row r="15" spans="2:29" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="9" t="s">
-        <v>35</v>
+        <v>66</v>
       </c>
       <c r="C15" s="9"/>
       <c r="D15" s="9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E15" s="9"/>
       <c r="F15" s="9" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="G15" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" s="9">
         <v>0</v>
@@ -2001,16 +2006,12 @@
     </row>
     <row r="16" spans="2:29" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="9" t="s">
-        <v>31</v>
+        <v>2</v>
       </c>
       <c r="C16" s="9"/>
-      <c r="D16" s="9" t="s">
-        <v>51</v>
-      </c>
+      <c r="D16" s="9"/>
       <c r="E16" s="9"/>
-      <c r="F16" s="9" t="s">
-        <v>58</v>
-      </c>
+      <c r="F16" s="9"/>
       <c r="G16" s="9">
         <v>0</v>
       </c>
@@ -2049,35 +2050,23 @@
       <c r="AB16" s="4"/>
       <c r="AC16" s="4"/>
     </row>
-    <row r="17" spans="2:29" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
+    <row r="17" spans="2:29" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="7">
+        <v>8</v>
+      </c>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
       <c r="F17" s="9"/>
-      <c r="G17" s="9">
-        <v>0</v>
-      </c>
-      <c r="H17" s="9">
-        <v>0</v>
-      </c>
-      <c r="I17" s="9">
-        <v>0</v>
-      </c>
-      <c r="J17" s="9">
-        <v>0</v>
-      </c>
-      <c r="K17" s="9">
-        <v>0</v>
-      </c>
-      <c r="L17" s="9">
-        <v>0</v>
-      </c>
-      <c r="M17" s="9">
-        <v>0</v>
-      </c>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
       <c r="N17" s="4"/>
       <c r="O17" s="4"/>
       <c r="P17" s="4"/>
@@ -2095,23 +2084,41 @@
       <c r="AB17" s="4"/>
       <c r="AC17" s="4"/>
     </row>
-    <row r="18" spans="2:29" ht="51" x14ac:dyDescent="0.25">
-      <c r="B18" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C18" s="7">
-        <v>8</v>
-      </c>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="8"/>
-      <c r="L18" s="8"/>
-      <c r="M18" s="8"/>
+    <row r="18" spans="2:29" ht="27" x14ac:dyDescent="0.25">
+      <c r="B18" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="G18" s="9">
+        <v>0</v>
+      </c>
+      <c r="H18" s="9">
+        <v>0</v>
+      </c>
+      <c r="I18" s="9">
+        <v>0</v>
+      </c>
+      <c r="J18" s="9">
+        <v>0</v>
+      </c>
+      <c r="K18" s="9">
+        <v>0</v>
+      </c>
+      <c r="L18" s="9">
+        <v>0</v>
+      </c>
+      <c r="M18" s="9">
+        <v>0</v>
+      </c>
       <c r="N18" s="4"/>
       <c r="O18" s="4"/>
       <c r="P18" s="4"/>
@@ -2131,17 +2138,15 @@
     </row>
     <row r="19" spans="2:29" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="9" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="C19" s="9"/>
       <c r="D19" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="E19" s="9" t="s">
-        <v>54</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="E19" s="9"/>
       <c r="F19" s="9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G19" s="9">
         <v>0</v>
@@ -2183,15 +2188,15 @@
     </row>
     <row r="20" spans="2:29" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="9" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C20" s="9"/>
       <c r="D20" s="9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E20" s="9"/>
       <c r="F20" s="9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G20" s="9">
         <v>0</v>
@@ -2233,16 +2238,12 @@
     </row>
     <row r="21" spans="2:29" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="9" t="s">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="C21" s="9"/>
-      <c r="D21" s="9" t="s">
-        <v>51</v>
-      </c>
+      <c r="D21" s="9"/>
       <c r="E21" s="9"/>
-      <c r="F21" s="9" t="s">
-        <v>58</v>
-      </c>
+      <c r="F21" s="9"/>
       <c r="G21" s="9">
         <v>0</v>
       </c>
@@ -2281,35 +2282,23 @@
       <c r="AB21" s="4"/>
       <c r="AC21" s="4"/>
     </row>
-    <row r="22" spans="2:29" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
+    <row r="22" spans="2:29" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="7">
+        <v>3</v>
+      </c>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
       <c r="F22" s="9"/>
-      <c r="G22" s="9">
-        <v>0</v>
-      </c>
-      <c r="H22" s="9">
-        <v>0</v>
-      </c>
-      <c r="I22" s="9">
-        <v>0</v>
-      </c>
-      <c r="J22" s="9">
-        <v>0</v>
-      </c>
-      <c r="K22" s="9">
-        <v>0</v>
-      </c>
-      <c r="L22" s="9">
-        <v>0</v>
-      </c>
-      <c r="M22" s="9">
-        <v>0</v>
-      </c>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="8"/>
+      <c r="M22" s="8"/>
       <c r="N22" s="4"/>
       <c r="O22" s="4"/>
       <c r="P22" s="4"/>
@@ -2327,23 +2316,41 @@
       <c r="AB22" s="4"/>
       <c r="AC22" s="4"/>
     </row>
-    <row r="23" spans="2:29" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="B23" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C23" s="7">
-        <v>3</v>
-      </c>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="8"/>
-      <c r="J23" s="8"/>
-      <c r="K23" s="8"/>
-      <c r="L23" s="8"/>
-      <c r="M23" s="8"/>
+    <row r="23" spans="2:29" ht="27" x14ac:dyDescent="0.25">
+      <c r="B23" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="G23" s="9">
+        <v>0</v>
+      </c>
+      <c r="H23" s="9">
+        <v>0</v>
+      </c>
+      <c r="I23" s="9">
+        <v>0</v>
+      </c>
+      <c r="J23" s="9">
+        <v>0</v>
+      </c>
+      <c r="K23" s="9">
+        <v>0</v>
+      </c>
+      <c r="L23" s="9">
+        <v>0</v>
+      </c>
+      <c r="M23" s="9">
+        <v>0</v>
+      </c>
       <c r="N23" s="4"/>
       <c r="O23" s="4"/>
       <c r="P23" s="4"/>
@@ -2363,17 +2370,15 @@
     </row>
     <row r="24" spans="2:29" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C24" s="9"/>
       <c r="D24" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="E24" s="9" t="s">
-        <v>54</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="E24" s="9"/>
       <c r="F24" s="9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G24" s="9">
         <v>0</v>
@@ -2415,16 +2420,12 @@
     </row>
     <row r="25" spans="2:29" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="9" t="s">
-        <v>39</v>
+        <v>2</v>
       </c>
       <c r="C25" s="9"/>
-      <c r="D25" s="9" t="s">
-        <v>51</v>
-      </c>
+      <c r="D25" s="9"/>
       <c r="E25" s="9"/>
-      <c r="F25" s="9" t="s">
-        <v>58</v>
-      </c>
+      <c r="F25" s="9"/>
       <c r="G25" s="9">
         <v>0</v>
       </c>
@@ -2509,35 +2510,23 @@
       <c r="AB26" s="4"/>
       <c r="AC26" s="4"/>
     </row>
-    <row r="27" spans="2:29" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="C27" s="9"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9"/>
+    <row r="27" spans="2:29" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" s="7">
+        <v>3</v>
+      </c>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
       <c r="F27" s="9"/>
-      <c r="G27" s="9">
-        <v>0</v>
-      </c>
-      <c r="H27" s="9">
-        <v>0</v>
-      </c>
-      <c r="I27" s="9">
-        <v>0</v>
-      </c>
-      <c r="J27" s="9">
-        <v>0</v>
-      </c>
-      <c r="K27" s="9">
-        <v>0</v>
-      </c>
-      <c r="L27" s="9">
-        <v>0</v>
-      </c>
-      <c r="M27" s="9">
-        <v>0</v>
-      </c>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="8"/>
+      <c r="K27" s="8"/>
+      <c r="L27" s="8"/>
+      <c r="M27" s="8"/>
       <c r="N27" s="4"/>
       <c r="O27" s="4"/>
       <c r="P27" s="4"/>
@@ -2555,23 +2544,41 @@
       <c r="AB27" s="4"/>
       <c r="AC27" s="4"/>
     </row>
-    <row r="28" spans="2:29" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="B28" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="C28" s="7">
-        <v>3</v>
-      </c>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
-      <c r="I28" s="8"/>
-      <c r="J28" s="8"/>
-      <c r="K28" s="8"/>
-      <c r="L28" s="8"/>
-      <c r="M28" s="8"/>
+    <row r="28" spans="2:29" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="B28" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="G28" s="9">
+        <v>0</v>
+      </c>
+      <c r="H28" s="9">
+        <v>0</v>
+      </c>
+      <c r="I28" s="9">
+        <v>0</v>
+      </c>
+      <c r="J28" s="9">
+        <v>0</v>
+      </c>
+      <c r="K28" s="9">
+        <v>0</v>
+      </c>
+      <c r="L28" s="9">
+        <v>0</v>
+      </c>
+      <c r="M28" s="9">
+        <v>0</v>
+      </c>
       <c r="N28" s="4"/>
       <c r="O28" s="4"/>
       <c r="P28" s="4"/>
@@ -2589,19 +2596,17 @@
       <c r="AB28" s="4"/>
       <c r="AC28" s="4"/>
     </row>
-    <row r="29" spans="2:29" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B29" s="9" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C29" s="9"/>
       <c r="D29" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="E29" s="9" t="s">
-        <v>55</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="E29" s="9"/>
       <c r="F29" s="9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G29" s="9">
         <v>0</v>
@@ -2643,16 +2648,12 @@
     </row>
     <row r="30" spans="2:29" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="9" t="s">
-        <v>39</v>
+        <v>2</v>
       </c>
       <c r="C30" s="9"/>
-      <c r="D30" s="9" t="s">
-        <v>51</v>
-      </c>
+      <c r="D30" s="9"/>
       <c r="E30" s="9"/>
-      <c r="F30" s="9" t="s">
-        <v>58</v>
-      </c>
+      <c r="F30" s="9"/>
       <c r="G30" s="9">
         <v>0</v>
       </c>
@@ -2738,34 +2739,24 @@
       <c r="AC31" s="4"/>
     </row>
     <row r="32" spans="2:29" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="C32" s="9"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="9"/>
-      <c r="F32" s="9"/>
-      <c r="G32" s="9">
-        <v>0</v>
-      </c>
-      <c r="H32" s="9">
-        <v>0</v>
-      </c>
-      <c r="I32" s="9">
-        <v>0</v>
-      </c>
-      <c r="J32" s="9">
-        <v>0</v>
-      </c>
-      <c r="K32" s="9">
-        <v>0</v>
-      </c>
-      <c r="L32" s="9">
-        <v>0</v>
-      </c>
-      <c r="M32" s="9">
-        <v>0</v>
-      </c>
+      <c r="B32" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C32" s="7">
+        <v>1</v>
+      </c>
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="G32" s="8"/>
+      <c r="H32" s="8"/>
+      <c r="I32" s="8"/>
+      <c r="J32" s="8"/>
+      <c r="K32" s="8"/>
+      <c r="L32" s="8"/>
+      <c r="M32" s="8"/>
       <c r="N32" s="4"/>
       <c r="O32" s="4"/>
       <c r="P32" s="4"/>
@@ -2783,23 +2774,39 @@
       <c r="AB32" s="4"/>
       <c r="AC32" s="4"/>
     </row>
-    <row r="33" spans="2:29" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B33" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C33" s="7">
+    <row r="33" spans="2:29" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="B33" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="G33" s="9">
         <v>1</v>
       </c>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="9"/>
-      <c r="G33" s="8"/>
-      <c r="H33" s="8"/>
-      <c r="I33" s="8"/>
-      <c r="J33" s="8"/>
-      <c r="K33" s="8"/>
-      <c r="L33" s="8"/>
-      <c r="M33" s="8"/>
+      <c r="H33" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="I33" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="J33" s="9">
+        <v>0</v>
+      </c>
+      <c r="K33" s="9">
+        <v>0</v>
+      </c>
+      <c r="L33" s="9">
+        <v>0</v>
+      </c>
+      <c r="M33" s="9">
+        <v>0</v>
+      </c>
       <c r="N33" s="4"/>
       <c r="O33" s="4"/>
       <c r="P33" s="4"/>
@@ -2817,39 +2824,25 @@
       <c r="AB33" s="4"/>
       <c r="AC33" s="4"/>
     </row>
-    <row r="34" spans="2:29" ht="40.5" x14ac:dyDescent="0.25">
-      <c r="B34" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="C34" s="9"/>
-      <c r="D34" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="E34" s="9"/>
+    <row r="34" spans="2:29" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="B34" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C34" s="7">
+        <v>3</v>
+      </c>
+      <c r="D34" s="8"/>
+      <c r="E34" s="8"/>
       <c r="F34" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="G34" s="9">
-        <v>1</v>
-      </c>
-      <c r="H34" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="I34" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="J34" s="9">
-        <v>0</v>
-      </c>
-      <c r="K34" s="9">
-        <v>0</v>
-      </c>
-      <c r="L34" s="9">
-        <v>0</v>
-      </c>
-      <c r="M34" s="9">
-        <v>0</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="G34" s="8"/>
+      <c r="H34" s="8"/>
+      <c r="I34" s="8"/>
+      <c r="J34" s="8"/>
+      <c r="K34" s="8"/>
+      <c r="L34" s="8"/>
+      <c r="M34" s="8"/>
       <c r="N34" s="4"/>
       <c r="O34" s="4"/>
       <c r="P34" s="4"/>
@@ -2867,15 +2860,17 @@
       <c r="AB34" s="4"/>
       <c r="AC34" s="4"/>
     </row>
-    <row r="35" spans="2:29" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:29" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="9" t="s">
-        <v>2</v>
+        <v>45</v>
       </c>
       <c r="C35" s="9"/>
-      <c r="D35" s="9"/>
+      <c r="D35" s="9" t="s">
+        <v>49</v>
+      </c>
       <c r="E35" s="9"/>
       <c r="F35" s="9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G35" s="9">
         <v>0</v>
@@ -2922,9 +2917,7 @@
       <c r="C36" s="9"/>
       <c r="D36" s="9"/>
       <c r="E36" s="9"/>
-      <c r="F36" s="9" t="s">
-        <v>58</v>
-      </c>
+      <c r="F36" s="9"/>
       <c r="G36" s="9">
         <v>0</v>
       </c>
@@ -2970,9 +2963,7 @@
       <c r="C37" s="9"/>
       <c r="D37" s="9"/>
       <c r="E37" s="9"/>
-      <c r="F37" s="9" t="s">
-        <v>58</v>
-      </c>
+      <c r="F37" s="9"/>
       <c r="G37" s="9">
         <v>0</v>
       </c>
@@ -3011,25 +3002,35 @@
       <c r="AB37" s="4"/>
       <c r="AC37" s="4"/>
     </row>
-    <row r="38" spans="2:29" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="B38" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="C38" s="7">
-        <v>3</v>
-      </c>
-      <c r="D38" s="8"/>
-      <c r="E38" s="8"/>
-      <c r="F38" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="G38" s="8"/>
-      <c r="H38" s="8"/>
-      <c r="I38" s="8"/>
-      <c r="J38" s="8"/>
-      <c r="K38" s="8"/>
-      <c r="L38" s="8"/>
-      <c r="M38" s="8"/>
+    <row r="38" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B38" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C38" s="9"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="9">
+        <v>0</v>
+      </c>
+      <c r="H38" s="9">
+        <v>0</v>
+      </c>
+      <c r="I38" s="9">
+        <v>0</v>
+      </c>
+      <c r="J38" s="9">
+        <v>0</v>
+      </c>
+      <c r="K38" s="9">
+        <v>0</v>
+      </c>
+      <c r="L38" s="9">
+        <v>0</v>
+      </c>
+      <c r="M38" s="9">
+        <v>0</v>
+      </c>
       <c r="N38" s="4"/>
       <c r="O38" s="4"/>
       <c r="P38" s="4"/>
@@ -3047,39 +3048,25 @@
       <c r="AB38" s="4"/>
       <c r="AC38" s="4"/>
     </row>
-    <row r="39" spans="2:29" ht="40.5" x14ac:dyDescent="0.25">
-      <c r="B39" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="C39" s="9"/>
-      <c r="D39" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="E39" s="9"/>
+    <row r="39" spans="2:29" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="B39" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C39" s="7">
+        <v>3</v>
+      </c>
+      <c r="D39" s="8"/>
+      <c r="E39" s="8"/>
       <c r="F39" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="G39" s="9">
-        <v>0</v>
-      </c>
-      <c r="H39" s="9">
-        <v>0</v>
-      </c>
-      <c r="I39" s="9">
-        <v>0</v>
-      </c>
-      <c r="J39" s="9">
-        <v>0</v>
-      </c>
-      <c r="K39" s="9">
-        <v>0</v>
-      </c>
-      <c r="L39" s="9">
-        <v>0</v>
-      </c>
-      <c r="M39" s="9">
-        <v>0</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="G39" s="8"/>
+      <c r="H39" s="8"/>
+      <c r="I39" s="8"/>
+      <c r="J39" s="8"/>
+      <c r="K39" s="8"/>
+      <c r="L39" s="8"/>
+      <c r="M39" s="8"/>
       <c r="N39" s="4"/>
       <c r="O39" s="4"/>
       <c r="P39" s="4"/>
@@ -3097,22 +3084,26 @@
       <c r="AB39" s="4"/>
       <c r="AC39" s="4"/>
     </row>
-    <row r="40" spans="2:29" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:29" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="9" t="s">
-        <v>2</v>
+        <v>60</v>
       </c>
       <c r="C40" s="9"/>
-      <c r="D40" s="9"/>
+      <c r="D40" s="9" t="s">
+        <v>49</v>
+      </c>
       <c r="E40" s="9"/>
-      <c r="F40" s="9"/>
+      <c r="F40" s="9" t="s">
+        <v>62</v>
+      </c>
       <c r="G40" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H40" s="9">
         <v>0</v>
       </c>
       <c r="I40" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J40" s="9">
         <v>0</v>
@@ -3143,22 +3134,26 @@
       <c r="AB40" s="4"/>
       <c r="AC40" s="4"/>
     </row>
-    <row r="41" spans="2:29" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:29" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C41" s="9"/>
+      <c r="D41" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E41" s="9"/>
+      <c r="F41" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="G41" s="9">
+        <v>3</v>
+      </c>
+      <c r="H41" s="9">
+        <v>0</v>
+      </c>
+      <c r="I41" s="9">
         <v>2</v>
-      </c>
-      <c r="C41" s="9"/>
-      <c r="D41" s="9"/>
-      <c r="E41" s="9"/>
-      <c r="F41" s="9"/>
-      <c r="G41" s="9">
-        <v>0</v>
-      </c>
-      <c r="H41" s="9">
-        <v>0</v>
-      </c>
-      <c r="I41" s="9">
-        <v>0</v>
       </c>
       <c r="J41" s="9">
         <v>0</v>
@@ -3189,22 +3184,26 @@
       <c r="AB41" s="4"/>
       <c r="AC41" s="4"/>
     </row>
-    <row r="42" spans="2:29" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:29" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="9" t="s">
-        <v>2</v>
+        <v>59</v>
       </c>
       <c r="C42" s="9"/>
-      <c r="D42" s="9"/>
+      <c r="D42" s="9" t="s">
+        <v>49</v>
+      </c>
       <c r="E42" s="9"/>
-      <c r="F42" s="9"/>
+      <c r="F42" s="9" t="s">
+        <v>62</v>
+      </c>
       <c r="G42" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H42" s="9">
         <v>0</v>
       </c>
       <c r="I42" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J42" s="9">
         <v>0</v>
@@ -3235,25 +3234,39 @@
       <c r="AB42" s="4"/>
       <c r="AC42" s="4"/>
     </row>
-    <row r="43" spans="2:29" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="B43" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C43" s="7">
-        <v>3</v>
-      </c>
-      <c r="D43" s="8"/>
-      <c r="E43" s="8"/>
+    <row r="43" spans="2:29" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="B43" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C43" s="9"/>
+      <c r="D43" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E43" s="9"/>
       <c r="F43" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="G43" s="8"/>
-      <c r="H43" s="8"/>
-      <c r="I43" s="8"/>
-      <c r="J43" s="8"/>
-      <c r="K43" s="8"/>
-      <c r="L43" s="8"/>
-      <c r="M43" s="8"/>
+        <v>62</v>
+      </c>
+      <c r="G43" s="9">
+        <v>2</v>
+      </c>
+      <c r="H43" s="9">
+        <v>0</v>
+      </c>
+      <c r="I43" s="9">
+        <v>4</v>
+      </c>
+      <c r="J43" s="9">
+        <v>0</v>
+      </c>
+      <c r="K43" s="9">
+        <v>0</v>
+      </c>
+      <c r="L43" s="9">
+        <v>0</v>
+      </c>
+      <c r="M43" s="9">
+        <v>0</v>
+      </c>
       <c r="N43" s="4"/>
       <c r="O43" s="4"/>
       <c r="P43" s="4"/>
@@ -3272,38 +3285,22 @@
       <c r="AC43" s="4"/>
     </row>
     <row r="44" spans="2:29" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="C44" s="9"/>
-      <c r="D44" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="E44" s="9"/>
-      <c r="F44" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="G44" s="9">
-        <v>1</v>
-      </c>
-      <c r="H44" s="9">
-        <v>0</v>
-      </c>
-      <c r="I44" s="9">
-        <v>1</v>
-      </c>
-      <c r="J44" s="9">
-        <v>0</v>
-      </c>
-      <c r="K44" s="9">
-        <v>0</v>
-      </c>
-      <c r="L44" s="9">
-        <v>0</v>
-      </c>
-      <c r="M44" s="9">
-        <v>0</v>
-      </c>
+      <c r="B44" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C44" s="7">
+        <v>3</v>
+      </c>
+      <c r="D44" s="8"/>
+      <c r="E44" s="8"/>
+      <c r="F44" s="9"/>
+      <c r="G44" s="8"/>
+      <c r="H44" s="8"/>
+      <c r="I44" s="8"/>
+      <c r="J44" s="8"/>
+      <c r="K44" s="8"/>
+      <c r="L44" s="8"/>
+      <c r="M44" s="8"/>
       <c r="N44" s="4"/>
       <c r="O44" s="4"/>
       <c r="P44" s="4"/>
@@ -3323,24 +3320,26 @@
     </row>
     <row r="45" spans="2:29" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="9" t="s">
-        <v>61</v>
+        <v>2</v>
       </c>
       <c r="C45" s="9"/>
       <c r="D45" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="E45" s="9"/>
+        <v>55</v>
+      </c>
+      <c r="E45" s="9" t="s">
+        <v>54</v>
+      </c>
       <c r="F45" s="9" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="G45" s="9">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H45" s="9">
         <v>0</v>
       </c>
       <c r="I45" s="9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J45" s="9">
         <v>0</v>
@@ -3373,24 +3372,20 @@
     </row>
     <row r="46" spans="2:29" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="9" t="s">
-        <v>62</v>
+        <v>2</v>
       </c>
       <c r="C46" s="9"/>
-      <c r="D46" s="9" t="s">
-        <v>51</v>
-      </c>
+      <c r="D46" s="9"/>
       <c r="E46" s="9"/>
-      <c r="F46" s="9" t="s">
-        <v>65</v>
-      </c>
+      <c r="F46" s="9"/>
       <c r="G46" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H46" s="9">
         <v>0</v>
       </c>
       <c r="I46" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J46" s="9">
         <v>0</v>
@@ -3423,16 +3418,12 @@
     </row>
     <row r="47" spans="2:29" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="9" t="s">
-        <v>64</v>
+        <v>2</v>
       </c>
       <c r="C47" s="9"/>
-      <c r="D47" s="9" t="s">
-        <v>51</v>
-      </c>
+      <c r="D47" s="9"/>
       <c r="E47" s="9"/>
-      <c r="F47" s="9" t="s">
-        <v>60</v>
-      </c>
+      <c r="F47" s="9"/>
       <c r="G47" s="9">
         <v>0</v>
       </c>
@@ -3471,23 +3462,37 @@
       <c r="AB47" s="4"/>
       <c r="AC47" s="4"/>
     </row>
-    <row r="48" spans="2:29" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B48" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C48" s="7">
-        <v>3</v>
-      </c>
-      <c r="D48" s="8"/>
-      <c r="E48" s="8"/>
-      <c r="F48" s="9"/>
-      <c r="G48" s="8"/>
-      <c r="H48" s="8"/>
-      <c r="I48" s="8"/>
-      <c r="J48" s="8"/>
-      <c r="K48" s="8"/>
-      <c r="L48" s="8"/>
-      <c r="M48" s="8"/>
+    <row r="48" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B48" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C48" s="9"/>
+      <c r="D48" s="9"/>
+      <c r="E48" s="9"/>
+      <c r="F48" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="G48" s="9">
+        <v>0</v>
+      </c>
+      <c r="H48" s="9">
+        <v>0</v>
+      </c>
+      <c r="I48" s="9">
+        <v>0</v>
+      </c>
+      <c r="J48" s="9">
+        <v>0</v>
+      </c>
+      <c r="K48" s="9">
+        <v>0</v>
+      </c>
+      <c r="L48" s="9">
+        <v>0</v>
+      </c>
+      <c r="M48" s="9">
+        <v>0</v>
+      </c>
       <c r="N48" s="4"/>
       <c r="O48" s="4"/>
       <c r="P48" s="4"/>
@@ -3506,38 +3511,39 @@
       <c r="AC48" s="4"/>
     </row>
     <row r="49" spans="2:29" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="C49" s="9"/>
-      <c r="D49" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="E49" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="F49" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="G49" s="9">
-        <v>0</v>
-      </c>
-      <c r="H49" s="9">
-        <v>0</v>
-      </c>
-      <c r="I49" s="9">
-        <v>0</v>
-      </c>
-      <c r="J49" s="9">
-        <v>0</v>
-      </c>
-      <c r="K49" s="9">
-        <v>0</v>
-      </c>
-      <c r="L49" s="9">
-        <v>0</v>
-      </c>
-      <c r="M49" s="9">
+      <c r="B49" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="5"/>
+      <c r="F49" s="5"/>
+      <c r="G49" s="5">
+        <f>SUM(G3:G48)</f>
+        <v>31</v>
+      </c>
+      <c r="H49" s="5">
+        <f>SUM(H4:H48)</f>
+        <v>0.5</v>
+      </c>
+      <c r="I49" s="5">
+        <f>SUM(I3:I48)</f>
+        <v>15.5</v>
+      </c>
+      <c r="J49" s="5">
+        <f>SUM(J3:J48)</f>
+        <v>0</v>
+      </c>
+      <c r="K49" s="5">
+        <f>SUM(K3:K48)</f>
+        <v>0</v>
+      </c>
+      <c r="L49" s="5">
+        <f>SUM(L3:L48)</f>
+        <v>0</v>
+      </c>
+      <c r="M49" s="5">
+        <f>SUM(M3:M48)</f>
         <v>0</v>
       </c>
       <c r="N49" s="4"/>
@@ -3558,34 +3564,18 @@
       <c r="AC49" s="4"/>
     </row>
     <row r="50" spans="2:29" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="C50" s="9"/>
-      <c r="D50" s="9"/>
-      <c r="E50" s="9"/>
-      <c r="F50" s="9"/>
-      <c r="G50" s="9">
-        <v>0</v>
-      </c>
-      <c r="H50" s="9">
-        <v>0</v>
-      </c>
-      <c r="I50" s="9">
-        <v>0</v>
-      </c>
-      <c r="J50" s="9">
-        <v>0</v>
-      </c>
-      <c r="K50" s="9">
-        <v>0</v>
-      </c>
-      <c r="L50" s="9">
-        <v>0</v>
-      </c>
-      <c r="M50" s="9">
-        <v>0</v>
-      </c>
+      <c r="B50" s="4"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="4"/>
+      <c r="E50" s="4"/>
+      <c r="F50" s="4"/>
+      <c r="G50" s="4"/>
+      <c r="H50" s="4"/>
+      <c r="I50" s="4"/>
+      <c r="J50" s="4"/>
+      <c r="K50" s="4"/>
+      <c r="L50" s="4"/>
+      <c r="M50" s="4"/>
       <c r="N50" s="4"/>
       <c r="O50" s="4"/>
       <c r="P50" s="4"/>
@@ -3604,34 +3594,18 @@
       <c r="AC50" s="4"/>
     </row>
     <row r="51" spans="2:29" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="C51" s="9"/>
-      <c r="D51" s="9"/>
-      <c r="E51" s="9"/>
-      <c r="F51" s="9"/>
-      <c r="G51" s="9">
-        <v>0</v>
-      </c>
-      <c r="H51" s="9">
-        <v>0</v>
-      </c>
-      <c r="I51" s="9">
-        <v>0</v>
-      </c>
-      <c r="J51" s="9">
-        <v>0</v>
-      </c>
-      <c r="K51" s="9">
-        <v>0</v>
-      </c>
-      <c r="L51" s="9">
-        <v>0</v>
-      </c>
-      <c r="M51" s="9">
-        <v>0</v>
-      </c>
+      <c r="B51" s="4"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="4"/>
+      <c r="E51" s="4"/>
+      <c r="F51" s="4"/>
+      <c r="G51" s="4"/>
+      <c r="H51" s="4"/>
+      <c r="I51" s="4"/>
+      <c r="J51" s="4"/>
+      <c r="K51" s="4"/>
+      <c r="L51" s="4"/>
+      <c r="M51" s="4"/>
       <c r="N51" s="4"/>
       <c r="O51" s="4"/>
       <c r="P51" s="4"/>
@@ -3650,36 +3624,18 @@
       <c r="AC51" s="4"/>
     </row>
     <row r="52" spans="2:29" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="C52" s="9"/>
-      <c r="D52" s="9"/>
-      <c r="E52" s="9"/>
-      <c r="F52" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="G52" s="9">
-        <v>0</v>
-      </c>
-      <c r="H52" s="9">
-        <v>0</v>
-      </c>
-      <c r="I52" s="9">
-        <v>0</v>
-      </c>
-      <c r="J52" s="9">
-        <v>0</v>
-      </c>
-      <c r="K52" s="9">
-        <v>0</v>
-      </c>
-      <c r="L52" s="9">
-        <v>0</v>
-      </c>
-      <c r="M52" s="9">
-        <v>0</v>
-      </c>
+      <c r="B52" s="4"/>
+      <c r="C52" s="1"/>
+      <c r="D52" s="4"/>
+      <c r="E52" s="4"/>
+      <c r="F52" s="4"/>
+      <c r="G52" s="4"/>
+      <c r="H52" s="4"/>
+      <c r="I52" s="4"/>
+      <c r="J52" s="4"/>
+      <c r="K52" s="4"/>
+      <c r="L52" s="4"/>
+      <c r="M52" s="4"/>
       <c r="N52" s="4"/>
       <c r="O52" s="4"/>
       <c r="P52" s="4"/>
@@ -3698,41 +3654,18 @@
       <c r="AC52" s="4"/>
     </row>
     <row r="53" spans="2:29" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C53" s="5"/>
-      <c r="D53" s="5"/>
-      <c r="E53" s="5"/>
-      <c r="F53" s="5"/>
-      <c r="G53" s="5">
-        <f>SUM(G3:G52)</f>
-        <v>26</v>
-      </c>
-      <c r="H53" s="5">
-        <f>SUM(H4:H52)</f>
-        <v>0.5</v>
-      </c>
-      <c r="I53" s="5">
-        <f>SUM(I3:I52)</f>
-        <v>11.5</v>
-      </c>
-      <c r="J53" s="5">
-        <f>SUM(J3:J52)</f>
-        <v>0</v>
-      </c>
-      <c r="K53" s="5">
-        <f>SUM(K3:K52)</f>
-        <v>0</v>
-      </c>
-      <c r="L53" s="5">
-        <f>SUM(L3:L52)</f>
-        <v>0</v>
-      </c>
-      <c r="M53" s="5">
-        <f>SUM(M3:M52)</f>
-        <v>0</v>
-      </c>
+      <c r="B53" s="4"/>
+      <c r="C53" s="1"/>
+      <c r="D53" s="4"/>
+      <c r="E53" s="4"/>
+      <c r="F53" s="4"/>
+      <c r="G53" s="4"/>
+      <c r="H53" s="4"/>
+      <c r="I53" s="4"/>
+      <c r="J53" s="4"/>
+      <c r="K53" s="4"/>
+      <c r="L53" s="4"/>
+      <c r="M53" s="4"/>
       <c r="N53" s="4"/>
       <c r="O53" s="4"/>
       <c r="P53" s="4"/>
@@ -6144,69 +6077,13 @@
       <c r="L144" s="4"/>
       <c r="M144" s="4"/>
     </row>
-    <row r="145" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B145" s="4"/>
-      <c r="C145" s="1"/>
-      <c r="D145" s="4"/>
-      <c r="E145" s="4"/>
-      <c r="F145" s="4"/>
-      <c r="G145" s="4"/>
-      <c r="H145" s="4"/>
-      <c r="I145" s="4"/>
-      <c r="J145" s="4"/>
-      <c r="K145" s="4"/>
-      <c r="L145" s="4"/>
-      <c r="M145" s="4"/>
-    </row>
-    <row r="146" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B146" s="4"/>
-      <c r="C146" s="1"/>
-      <c r="D146" s="4"/>
-      <c r="E146" s="4"/>
-      <c r="F146" s="4"/>
-      <c r="G146" s="4"/>
-      <c r="H146" s="4"/>
-      <c r="I146" s="4"/>
-      <c r="J146" s="4"/>
-      <c r="K146" s="4"/>
-      <c r="L146" s="4"/>
-      <c r="M146" s="4"/>
-    </row>
-    <row r="147" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B147" s="4"/>
-      <c r="C147" s="1"/>
-      <c r="D147" s="4"/>
-      <c r="E147" s="4"/>
-      <c r="F147" s="4"/>
-      <c r="G147" s="4"/>
-      <c r="H147" s="4"/>
-      <c r="I147" s="4"/>
-      <c r="J147" s="4"/>
-      <c r="K147" s="4"/>
-      <c r="L147" s="4"/>
-      <c r="M147" s="4"/>
-    </row>
-    <row r="148" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B148" s="4"/>
-      <c r="C148" s="1"/>
-      <c r="D148" s="4"/>
-      <c r="E148" s="4"/>
-      <c r="F148" s="4"/>
-      <c r="G148" s="4"/>
-      <c r="H148" s="4"/>
-      <c r="I148" s="4"/>
-      <c r="J148" s="4"/>
-      <c r="K148" s="4"/>
-      <c r="L148" s="4"/>
-      <c r="M148" s="4"/>
-    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:W1"/>
   </mergeCells>
   <pageMargins left="0.3" right="0.3" top="0.3" bottom="0.3" header="0" footer="0"/>
-  <pageSetup scale="45" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
-  <drawing r:id="rId1"/>
+  <pageSetup scale="45" fitToHeight="0" orientation="landscape" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Moved user story 8 into dev
</commit_message>
<xml_diff>
--- a/Sprint 2/Sprint_Backlog/Sprint2Backlog.xlsx
+++ b/Sprint 2/Sprint_Backlog/Sprint2Backlog.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22325"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\afzalmiah\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\The king\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2465C009-8FD1-448B-B00C-9B694F161422}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" tabRatio="500"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Agile Sprint Backlog" sheetId="5" r:id="rId1"/>
@@ -20,12 +21,14 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Agile Sprint Backlog'!$B$2:$W$28</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Agile Sprint Backlog - BLANK'!$B$2:$V$28</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="68">
   <si>
     <t>User Story #1</t>
   </si>
@@ -235,11 +238,14 @@
   <si>
     <t xml:space="preserve">2. Display the result received back to the user. </t>
   </si>
+  <si>
+    <t>In development</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -421,7 +427,7 @@
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -483,7 +489,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -534,7 +539,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>31</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.5</c:v>
@@ -1287,7 +1292,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
     <pageSetUpPr fitToPage="1"/>
@@ -1295,8 +1300,8 @@
   <dimension ref="B1:AC144"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B36" sqref="B36"/>
+      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -2834,7 +2839,7 @@
       <c r="D34" s="8"/>
       <c r="E34" s="8"/>
       <c r="F34" s="9" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="G34" s="8"/>
       <c r="H34" s="8"/>
@@ -2870,10 +2875,10 @@
       </c>
       <c r="E35" s="9"/>
       <c r="F35" s="9" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="G35" s="9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H35" s="9">
         <v>0</v>
@@ -3520,7 +3525,7 @@
       <c r="F49" s="5"/>
       <c r="G49" s="5">
         <f>SUM(G3:G48)</f>
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="H49" s="5">
         <f>SUM(H4:H48)</f>
@@ -6088,7 +6093,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="3" tint="0.39997558519241921"/>
     <pageSetUpPr fitToPage="1"/>
@@ -9793,7 +9798,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="1"/>
   </sheetPr>

</xml_diff>

<commit_message>
Final Version of Sprint Backlog 2.
Burndown Chart is in a separate file called BurnDownChartSprint2 as the BurnDown Chart in the Sprint Backlog 2 was not working.
</commit_message>
<xml_diff>
--- a/Sprint 2/Sprint_Backlog/Sprint2Backlog.xlsx
+++ b/Sprint 2/Sprint_Backlog/Sprint2Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arnav\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{458E6161-8319-4D74-8D49-CB29DDDD0D83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D201DBFC-47D4-467E-8558-1357CBD99292}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="65">
   <si>
     <t>User Story #1</t>
   </si>
@@ -230,9 +230,6 @@
   <si>
     <t xml:space="preserve">Clsoed </t>
   </si>
-  <si>
-    <t>Not Started</t>
-  </si>
 </sst>
 </file>
 
@@ -399,7 +396,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -511,22 +508,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>51</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>16.5</c:v>
+                  <c:v>18.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -1628,7 +1625,7 @@
         <v>4</v>
       </c>
       <c r="K8" s="9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L8" s="9">
         <v>0</v>
@@ -1678,7 +1675,7 @@
         <v>4</v>
       </c>
       <c r="K9" s="9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L9" s="9">
         <v>0</v>
@@ -1728,7 +1725,7 @@
         <v>0</v>
       </c>
       <c r="K10" s="9">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L10" s="9">
         <v>0</v>
@@ -1811,7 +1808,7 @@
         <v>0</v>
       </c>
       <c r="J12" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K12" s="9">
         <v>0</v>
@@ -1950,7 +1947,7 @@
         <v>0</v>
       </c>
       <c r="K15" s="9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L15" s="9">
         <v>0</v>
@@ -2085,10 +2082,10 @@
         <v>0</v>
       </c>
       <c r="J18" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K18" s="9">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L18" s="9">
         <v>0</v>
@@ -2448,10 +2445,10 @@
         <v>0</v>
       </c>
       <c r="K26" s="9">
+        <v>4</v>
+      </c>
+      <c r="L26" s="9">
         <v>2</v>
-      </c>
-      <c r="L26" s="9">
-        <v>0</v>
       </c>
       <c r="M26" s="9">
         <v>0</v>
@@ -2578,7 +2575,7 @@
         <v>0</v>
       </c>
       <c r="I29" s="9">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J29" s="9">
         <v>0</v>
@@ -2755,10 +2752,10 @@
         <v>50</v>
       </c>
       <c r="F33" s="9" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G33" s="9">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H33" s="9">
         <v>0</v>
@@ -2773,7 +2770,7 @@
         <v>0</v>
       </c>
       <c r="L33" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M33" s="9">
         <v>0</v>
@@ -2805,7 +2802,7 @@
       <c r="F34" s="5"/>
       <c r="G34" s="5">
         <f>SUM(G3:G33)</f>
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="H34" s="5">
         <f>SUM(H4:H33)</f>
@@ -2813,7 +2810,7 @@
       </c>
       <c r="I34" s="5">
         <f>SUM(I3:I33)</f>
-        <v>16.5</v>
+        <v>18.5</v>
       </c>
       <c r="J34" s="5">
         <f>SUM(J3:J33)</f>
@@ -2821,11 +2818,11 @@
       </c>
       <c r="K34" s="5">
         <f>SUM(K3:K33)</f>
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="L34" s="5">
         <f>SUM(L3:L33)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M34" s="5">
         <f>SUM(M3:M33)</f>

</xml_diff>